<commit_message>
tab con destinazioni usate non in 200
</commit_message>
<xml_diff>
--- a/test/crawl-new-website.xlsx
+++ b/test/crawl-new-website.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cervedgroup-my.sharepoint.com/personal/carlo_sefcek_cerved_com/Documents/Carlo/Python/PythonSEO/redirect-mapper-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{4BAE5168-DBD6-4D52-9EA5-74371E1DD103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF052461-B8B0-443F-A2F7-2630FCA65468}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{4BAE5168-DBD6-4D52-9EA5-74371E1DD103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F04244B-1FAC-481A-89A7-A64BBC6D495A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EB465845-177C-4413-96B4-920549546B26}"/>
   </bookViews>
   <sheets>
     <sheet name="crawl" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">crawl!$A$1:$B$299</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -408,10 +411,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -434,13 +445,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -773,11 +788,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803EFE23-58C0-4A38-A592-4F07A8E9A009}">
-  <dimension ref="A1:B299"/>
+  <dimension ref="A1:B304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="B300" sqref="B300"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -797,7 +810,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>200</v>
       </c>
     </row>
@@ -805,7 +818,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>200</v>
       </c>
     </row>
@@ -813,7 +826,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>200</v>
       </c>
     </row>
@@ -821,7 +834,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>200</v>
       </c>
     </row>
@@ -829,7 +842,7 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>200</v>
       </c>
     </row>
@@ -837,7 +850,7 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>200</v>
       </c>
     </row>
@@ -845,7 +858,7 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>200</v>
       </c>
     </row>
@@ -853,7 +866,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>200</v>
       </c>
     </row>
@@ -861,7 +874,7 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>200</v>
       </c>
     </row>
@@ -869,7 +882,7 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>200</v>
       </c>
     </row>
@@ -877,7 +890,7 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>200</v>
       </c>
     </row>
@@ -885,15 +898,15 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>200</v>
+      <c r="B13" s="1">
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>200</v>
       </c>
     </row>
@@ -901,7 +914,7 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>200</v>
       </c>
     </row>
@@ -909,7 +922,7 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>200</v>
       </c>
     </row>
@@ -917,15 +930,15 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>200</v>
+      <c r="B17" s="1">
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>200</v>
       </c>
     </row>
@@ -933,7 +946,7 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>200</v>
       </c>
     </row>
@@ -941,7 +954,7 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>200</v>
       </c>
     </row>
@@ -949,15 +962,15 @@
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>200</v>
+      <c r="B21" s="1">
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>200</v>
       </c>
     </row>
@@ -965,7 +978,7 @@
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>200</v>
       </c>
     </row>
@@ -973,15 +986,15 @@
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>200</v>
+      <c r="B24" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>200</v>
       </c>
     </row>
@@ -989,7 +1002,7 @@
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>200</v>
       </c>
     </row>
@@ -997,7 +1010,7 @@
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1005,7 +1018,7 @@
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1013,7 +1026,7 @@
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1021,7 +1034,7 @@
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1029,7 +1042,7 @@
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1037,7 +1050,7 @@
       <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1045,7 +1058,7 @@
       <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1053,7 +1066,7 @@
       <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1061,7 +1074,7 @@
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1069,7 +1082,7 @@
       <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1077,7 +1090,7 @@
       <c r="A37" t="s">
         <v>34</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1085,7 +1098,7 @@
       <c r="A38" t="s">
         <v>35</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1093,7 +1106,7 @@
       <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1101,7 +1114,7 @@
       <c r="A40" t="s">
         <v>30</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1109,7 +1122,7 @@
       <c r="A41" t="s">
         <v>31</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1117,7 +1130,7 @@
       <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1125,7 +1138,7 @@
       <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1133,7 +1146,7 @@
       <c r="A44" t="s">
         <v>39</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1141,7 +1154,7 @@
       <c r="A45" t="s">
         <v>40</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1149,7 +1162,7 @@
       <c r="A46" t="s">
         <v>41</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1157,7 +1170,7 @@
       <c r="A47" t="s">
         <v>42</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1165,7 +1178,7 @@
       <c r="A48" t="s">
         <v>43</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1173,7 +1186,7 @@
       <c r="A49" t="s">
         <v>43</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1181,7 +1194,7 @@
       <c r="A50" t="s">
         <v>44</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1189,7 +1202,7 @@
       <c r="A51" t="s">
         <v>44</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1197,7 +1210,7 @@
       <c r="A52" t="s">
         <v>45</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1205,7 +1218,7 @@
       <c r="A53" t="s">
         <v>45</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1213,7 +1226,7 @@
       <c r="A54" t="s">
         <v>46</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1221,7 +1234,7 @@
       <c r="A55" t="s">
         <v>46</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1229,7 +1242,7 @@
       <c r="A56" t="s">
         <v>43</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1237,7 +1250,7 @@
       <c r="A57" t="s">
         <v>43</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1245,7 +1258,7 @@
       <c r="A58" t="s">
         <v>47</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1253,7 +1266,7 @@
       <c r="A59" t="s">
         <v>48</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1261,7 +1274,7 @@
       <c r="A60" t="s">
         <v>49</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1269,7 +1282,7 @@
       <c r="A61" t="s">
         <v>50</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1277,7 +1290,7 @@
       <c r="A62" t="s">
         <v>51</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1285,7 +1298,7 @@
       <c r="A63" t="s">
         <v>52</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1293,7 +1306,7 @@
       <c r="A64" t="s">
         <v>53</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1301,7 +1314,7 @@
       <c r="A65" t="s">
         <v>54</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1309,15 +1322,15 @@
       <c r="A66" t="s">
         <v>55</v>
       </c>
-      <c r="B66">
-        <v>200</v>
+      <c r="B66" s="1">
+        <v>301</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>56</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1325,7 +1338,7 @@
       <c r="A68" t="s">
         <v>52</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1333,7 +1346,7 @@
       <c r="A69" t="s">
         <v>57</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1341,7 +1354,7 @@
       <c r="A70" t="s">
         <v>57</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1349,7 +1362,7 @@
       <c r="A71" t="s">
         <v>58</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1357,7 +1370,7 @@
       <c r="A72" t="s">
         <v>59</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1365,7 +1378,7 @@
       <c r="A73" t="s">
         <v>60</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1373,7 +1386,7 @@
       <c r="A74" t="s">
         <v>61</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1381,7 +1394,7 @@
       <c r="A75" t="s">
         <v>62</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1389,7 +1402,7 @@
       <c r="A76" t="s">
         <v>62</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1397,7 +1410,7 @@
       <c r="A77" t="s">
         <v>63</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1405,7 +1418,7 @@
       <c r="A78" t="s">
         <v>64</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1413,7 +1426,7 @@
       <c r="A79" t="s">
         <v>65</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1421,7 +1434,7 @@
       <c r="A80" t="s">
         <v>66</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1429,7 +1442,7 @@
       <c r="A81" t="s">
         <v>67</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1437,7 +1450,7 @@
       <c r="A82" t="s">
         <v>68</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1445,7 +1458,7 @@
       <c r="A83" t="s">
         <v>69</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1453,7 +1466,7 @@
       <c r="A84" t="s">
         <v>70</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1461,7 +1474,7 @@
       <c r="A85" t="s">
         <v>71</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1469,7 +1482,7 @@
       <c r="A86" t="s">
         <v>72</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1477,7 +1490,7 @@
       <c r="A87" t="s">
         <v>73</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1485,7 +1498,7 @@
       <c r="A88" t="s">
         <v>74</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1493,7 +1506,7 @@
       <c r="A89" t="s">
         <v>75</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1501,7 +1514,7 @@
       <c r="A90" t="s">
         <v>76</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1509,7 +1522,7 @@
       <c r="A91" t="s">
         <v>77</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1517,7 +1530,7 @@
       <c r="A92" t="s">
         <v>78</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1525,7 +1538,7 @@
       <c r="A93" t="s">
         <v>79</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1533,7 +1546,7 @@
       <c r="A94" t="s">
         <v>36</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1541,7 +1554,7 @@
       <c r="A95" t="s">
         <v>43</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1549,7 +1562,7 @@
       <c r="A96" t="s">
         <v>80</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1557,7 +1570,7 @@
       <c r="A97" t="s">
         <v>81</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1565,7 +1578,7 @@
       <c r="A98" t="s">
         <v>82</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1573,7 +1586,7 @@
       <c r="A99" t="s">
         <v>83</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1581,7 +1594,7 @@
       <c r="A100" t="s">
         <v>84</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1589,7 +1602,7 @@
       <c r="A101" t="s">
         <v>85</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1597,7 +1610,7 @@
       <c r="A102" t="s">
         <v>86</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1605,7 +1618,7 @@
       <c r="A103" t="s">
         <v>87</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1613,7 +1626,7 @@
       <c r="A104" t="s">
         <v>56</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1621,7 +1634,7 @@
       <c r="A105" t="s">
         <v>88</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1629,7 +1642,7 @@
       <c r="A106" t="s">
         <v>89</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1637,7 +1650,7 @@
       <c r="A107" t="s">
         <v>89</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1645,7 +1658,7 @@
       <c r="A108" t="s">
         <v>88</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1653,7 +1666,7 @@
       <c r="A109" t="s">
         <v>90</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1661,7 +1674,7 @@
       <c r="A110" t="s">
         <v>88</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1669,7 +1682,7 @@
       <c r="A111" t="s">
         <v>91</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1677,7 +1690,7 @@
       <c r="A112" t="s">
         <v>91</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1685,7 +1698,7 @@
       <c r="A113" t="s">
         <v>92</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1693,7 +1706,7 @@
       <c r="A114" t="s">
         <v>92</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1701,7 +1714,7 @@
       <c r="A115" t="s">
         <v>92</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1709,7 +1722,7 @@
       <c r="A116" t="s">
         <v>92</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1717,7 +1730,7 @@
       <c r="A117" t="s">
         <v>93</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1725,7 +1738,7 @@
       <c r="A118" t="s">
         <v>94</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1733,7 +1746,7 @@
       <c r="A119" t="s">
         <v>94</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1741,7 +1754,7 @@
       <c r="A120" t="s">
         <v>93</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1749,7 +1762,7 @@
       <c r="A121" t="s">
         <v>95</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1757,7 +1770,7 @@
       <c r="A122" t="s">
         <v>96</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1765,7 +1778,7 @@
       <c r="A123" t="s">
         <v>97</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1773,7 +1786,7 @@
       <c r="A124" t="s">
         <v>98</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1781,7 +1794,7 @@
       <c r="A125" t="s">
         <v>99</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1789,7 +1802,7 @@
       <c r="A126" t="s">
         <v>100</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1797,7 +1810,7 @@
       <c r="A127" t="s">
         <v>101</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1805,7 +1818,7 @@
       <c r="A128" t="s">
         <v>102</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1813,7 +1826,7 @@
       <c r="A129" t="s">
         <v>103</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1821,7 +1834,7 @@
       <c r="A130" t="s">
         <v>104</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1829,7 +1842,7 @@
       <c r="A131" t="s">
         <v>104</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1837,7 +1850,7 @@
       <c r="A132" t="s">
         <v>105</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1845,7 +1858,7 @@
       <c r="A133" t="s">
         <v>106</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1853,7 +1866,7 @@
       <c r="A134" t="s">
         <v>72</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1861,7 +1874,7 @@
       <c r="A135" t="s">
         <v>107</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1869,7 +1882,7 @@
       <c r="A136" t="s">
         <v>108</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1877,7 +1890,7 @@
       <c r="A137" t="s">
         <v>109</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1885,7 +1898,7 @@
       <c r="A138" t="s">
         <v>110</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1893,7 +1906,7 @@
       <c r="A139" t="s">
         <v>111</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1901,7 +1914,7 @@
       <c r="A140" t="s">
         <v>112</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1909,7 +1922,7 @@
       <c r="A141" t="s">
         <v>113</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1917,7 +1930,7 @@
       <c r="A142" t="s">
         <v>114</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1925,7 +1938,7 @@
       <c r="A143" t="s">
         <v>115</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1933,7 +1946,7 @@
       <c r="A144" t="s">
         <v>116</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1941,7 +1954,7 @@
       <c r="A145" t="s">
         <v>117</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1949,7 +1962,7 @@
       <c r="A146" t="s">
         <v>118</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1957,7 +1970,7 @@
       <c r="A147" t="s">
         <v>117</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1965,7 +1978,7 @@
       <c r="A148" t="s">
         <v>118</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1973,7 +1986,7 @@
       <c r="A149" t="s">
         <v>119</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1981,7 +1994,7 @@
       <c r="A150" t="s">
         <v>2</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1989,7 +2002,7 @@
       <c r="A151" t="s">
         <v>3</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="1">
         <v>200</v>
       </c>
     </row>
@@ -1997,7 +2010,7 @@
       <c r="A152" t="s">
         <v>3</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2005,7 +2018,7 @@
       <c r="A153" t="s">
         <v>4</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2013,7 +2026,7 @@
       <c r="A154" t="s">
         <v>5</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2021,7 +2034,7 @@
       <c r="A155" t="s">
         <v>6</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2029,7 +2042,7 @@
       <c r="A156" t="s">
         <v>7</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2037,7 +2050,7 @@
       <c r="A157" t="s">
         <v>8</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2045,7 +2058,7 @@
       <c r="A158" t="s">
         <v>8</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2053,7 +2066,7 @@
       <c r="A159" t="s">
         <v>9</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2061,7 +2074,7 @@
       <c r="A160" t="s">
         <v>10</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2069,7 +2082,7 @@
       <c r="A161" t="s">
         <v>11</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2077,7 +2090,7 @@
       <c r="A162" t="s">
         <v>12</v>
       </c>
-      <c r="B162">
+      <c r="B162" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2085,7 +2098,7 @@
       <c r="A163" t="s">
         <v>13</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2093,7 +2106,7 @@
       <c r="A164" t="s">
         <v>14</v>
       </c>
-      <c r="B164">
+      <c r="B164" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2101,7 +2114,7 @@
       <c r="A165" t="s">
         <v>15</v>
       </c>
-      <c r="B165">
+      <c r="B165" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2109,7 +2122,7 @@
       <c r="A166" t="s">
         <v>16</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2117,7 +2130,7 @@
       <c r="A167" t="s">
         <v>17</v>
       </c>
-      <c r="B167">
+      <c r="B167" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2125,7 +2138,7 @@
       <c r="A168" t="s">
         <v>18</v>
       </c>
-      <c r="B168">
+      <c r="B168" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2133,7 +2146,7 @@
       <c r="A169" t="s">
         <v>19</v>
       </c>
-      <c r="B169">
+      <c r="B169" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2141,7 +2154,7 @@
       <c r="A170" t="s">
         <v>20</v>
       </c>
-      <c r="B170">
+      <c r="B170" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2149,7 +2162,7 @@
       <c r="A171" t="s">
         <v>21</v>
       </c>
-      <c r="B171">
+      <c r="B171" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2157,7 +2170,7 @@
       <c r="A172" t="s">
         <v>22</v>
       </c>
-      <c r="B172">
+      <c r="B172" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2165,7 +2178,7 @@
       <c r="A173" t="s">
         <v>23</v>
       </c>
-      <c r="B173">
+      <c r="B173" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2173,7 +2186,7 @@
       <c r="A174" t="s">
         <v>24</v>
       </c>
-      <c r="B174">
+      <c r="B174" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2181,7 +2194,7 @@
       <c r="A175" t="s">
         <v>25</v>
       </c>
-      <c r="B175">
+      <c r="B175" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2189,7 +2202,7 @@
       <c r="A176" t="s">
         <v>26</v>
       </c>
-      <c r="B176">
+      <c r="B176" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2197,7 +2210,7 @@
       <c r="A177" t="s">
         <v>27</v>
       </c>
-      <c r="B177">
+      <c r="B177" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2205,7 +2218,7 @@
       <c r="A178" t="s">
         <v>28</v>
       </c>
-      <c r="B178">
+      <c r="B178" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2213,7 +2226,7 @@
       <c r="A179" t="s">
         <v>28</v>
       </c>
-      <c r="B179">
+      <c r="B179" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2221,7 +2234,7 @@
       <c r="A180" t="s">
         <v>29</v>
       </c>
-      <c r="B180">
+      <c r="B180" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2229,7 +2242,7 @@
       <c r="A181" t="s">
         <v>30</v>
       </c>
-      <c r="B181">
+      <c r="B181" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2237,7 +2250,7 @@
       <c r="A182" t="s">
         <v>31</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2245,7 +2258,7 @@
       <c r="A183" t="s">
         <v>32</v>
       </c>
-      <c r="B183">
+      <c r="B183" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2253,7 +2266,7 @@
       <c r="A184" t="s">
         <v>33</v>
       </c>
-      <c r="B184">
+      <c r="B184" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2261,7 +2274,7 @@
       <c r="A185" t="s">
         <v>34</v>
       </c>
-      <c r="B185">
+      <c r="B185" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2269,7 +2282,7 @@
       <c r="A186" t="s">
         <v>35</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2277,7 +2290,7 @@
       <c r="A187" t="s">
         <v>36</v>
       </c>
-      <c r="B187">
+      <c r="B187" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2285,7 +2298,7 @@
       <c r="A188" t="s">
         <v>30</v>
       </c>
-      <c r="B188">
+      <c r="B188" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2293,7 +2306,7 @@
       <c r="A189" t="s">
         <v>31</v>
       </c>
-      <c r="B189">
+      <c r="B189" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2301,7 +2314,7 @@
       <c r="A190" t="s">
         <v>37</v>
       </c>
-      <c r="B190">
+      <c r="B190" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2309,7 +2322,7 @@
       <c r="A191" t="s">
         <v>38</v>
       </c>
-      <c r="B191">
+      <c r="B191" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2317,7 +2330,7 @@
       <c r="A192" t="s">
         <v>39</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2325,7 +2338,7 @@
       <c r="A193" t="s">
         <v>40</v>
       </c>
-      <c r="B193">
+      <c r="B193" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2333,7 +2346,7 @@
       <c r="A194" t="s">
         <v>41</v>
       </c>
-      <c r="B194">
+      <c r="B194" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2341,7 +2354,7 @@
       <c r="A195" t="s">
         <v>42</v>
       </c>
-      <c r="B195">
+      <c r="B195" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2349,7 +2362,7 @@
       <c r="A196" t="s">
         <v>43</v>
       </c>
-      <c r="B196">
+      <c r="B196" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2357,7 +2370,7 @@
       <c r="A197" t="s">
         <v>43</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2365,7 +2378,7 @@
       <c r="A198" t="s">
         <v>44</v>
       </c>
-      <c r="B198">
+      <c r="B198" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2373,7 +2386,7 @@
       <c r="A199" t="s">
         <v>44</v>
       </c>
-      <c r="B199">
+      <c r="B199" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2381,7 +2394,7 @@
       <c r="A200" t="s">
         <v>45</v>
       </c>
-      <c r="B200">
+      <c r="B200" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2389,7 +2402,7 @@
       <c r="A201" t="s">
         <v>45</v>
       </c>
-      <c r="B201">
+      <c r="B201" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2397,7 +2410,7 @@
       <c r="A202" t="s">
         <v>46</v>
       </c>
-      <c r="B202">
+      <c r="B202" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2405,7 +2418,7 @@
       <c r="A203" t="s">
         <v>46</v>
       </c>
-      <c r="B203">
+      <c r="B203" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2413,7 +2426,7 @@
       <c r="A204" t="s">
         <v>43</v>
       </c>
-      <c r="B204">
+      <c r="B204" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2421,7 +2434,7 @@
       <c r="A205" t="s">
         <v>43</v>
       </c>
-      <c r="B205">
+      <c r="B205" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2429,7 +2442,7 @@
       <c r="A206" t="s">
         <v>47</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2437,7 +2450,7 @@
       <c r="A207" t="s">
         <v>48</v>
       </c>
-      <c r="B207">
+      <c r="B207" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2445,7 +2458,7 @@
       <c r="A208" t="s">
         <v>49</v>
       </c>
-      <c r="B208">
+      <c r="B208" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2453,7 +2466,7 @@
       <c r="A209" t="s">
         <v>50</v>
       </c>
-      <c r="B209">
+      <c r="B209" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2461,7 +2474,7 @@
       <c r="A210" t="s">
         <v>51</v>
       </c>
-      <c r="B210">
+      <c r="B210" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2469,7 +2482,7 @@
       <c r="A211" t="s">
         <v>52</v>
       </c>
-      <c r="B211">
+      <c r="B211" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2477,7 +2490,7 @@
       <c r="A212" t="s">
         <v>53</v>
       </c>
-      <c r="B212">
+      <c r="B212" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2485,7 +2498,7 @@
       <c r="A213" t="s">
         <v>54</v>
       </c>
-      <c r="B213">
+      <c r="B213" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2493,15 +2506,15 @@
       <c r="A214" t="s">
         <v>55</v>
       </c>
-      <c r="B214">
-        <v>200</v>
+      <c r="B214" s="1">
+        <v>301</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>56</v>
       </c>
-      <c r="B215">
+      <c r="B215" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2509,7 +2522,7 @@
       <c r="A216" t="s">
         <v>52</v>
       </c>
-      <c r="B216">
+      <c r="B216" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2517,7 +2530,7 @@
       <c r="A217" t="s">
         <v>57</v>
       </c>
-      <c r="B217">
+      <c r="B217" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2525,7 +2538,7 @@
       <c r="A218" t="s">
         <v>57</v>
       </c>
-      <c r="B218">
+      <c r="B218" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2533,7 +2546,7 @@
       <c r="A219" t="s">
         <v>58</v>
       </c>
-      <c r="B219">
+      <c r="B219" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2541,7 +2554,7 @@
       <c r="A220" t="s">
         <v>59</v>
       </c>
-      <c r="B220">
+      <c r="B220" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2549,7 +2562,7 @@
       <c r="A221" t="s">
         <v>60</v>
       </c>
-      <c r="B221">
+      <c r="B221" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2557,7 +2570,7 @@
       <c r="A222" t="s">
         <v>61</v>
       </c>
-      <c r="B222">
+      <c r="B222" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2565,7 +2578,7 @@
       <c r="A223" t="s">
         <v>62</v>
       </c>
-      <c r="B223">
+      <c r="B223" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2573,7 +2586,7 @@
       <c r="A224" t="s">
         <v>62</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2581,7 +2594,7 @@
       <c r="A225" t="s">
         <v>63</v>
       </c>
-      <c r="B225">
+      <c r="B225" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2589,7 +2602,7 @@
       <c r="A226" t="s">
         <v>64</v>
       </c>
-      <c r="B226">
+      <c r="B226" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2597,7 +2610,7 @@
       <c r="A227" t="s">
         <v>65</v>
       </c>
-      <c r="B227">
+      <c r="B227" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2605,7 +2618,7 @@
       <c r="A228" t="s">
         <v>66</v>
       </c>
-      <c r="B228">
+      <c r="B228" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2613,7 +2626,7 @@
       <c r="A229" t="s">
         <v>67</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2621,7 +2634,7 @@
       <c r="A230" t="s">
         <v>68</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2629,7 +2642,7 @@
       <c r="A231" t="s">
         <v>69</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2637,7 +2650,7 @@
       <c r="A232" t="s">
         <v>70</v>
       </c>
-      <c r="B232">
+      <c r="B232" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2645,7 +2658,7 @@
       <c r="A233" t="s">
         <v>71</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2653,7 +2666,7 @@
       <c r="A234" t="s">
         <v>72</v>
       </c>
-      <c r="B234">
+      <c r="B234" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2661,7 +2674,7 @@
       <c r="A235" t="s">
         <v>73</v>
       </c>
-      <c r="B235">
+      <c r="B235" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2669,7 +2682,7 @@
       <c r="A236" t="s">
         <v>74</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2677,7 +2690,7 @@
       <c r="A237" t="s">
         <v>75</v>
       </c>
-      <c r="B237">
+      <c r="B237" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2685,7 +2698,7 @@
       <c r="A238" t="s">
         <v>76</v>
       </c>
-      <c r="B238">
+      <c r="B238" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2693,7 +2706,7 @@
       <c r="A239" t="s">
         <v>77</v>
       </c>
-      <c r="B239">
+      <c r="B239" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2701,7 +2714,7 @@
       <c r="A240" t="s">
         <v>78</v>
       </c>
-      <c r="B240">
+      <c r="B240" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2709,7 +2722,7 @@
       <c r="A241" t="s">
         <v>79</v>
       </c>
-      <c r="B241">
+      <c r="B241" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2717,7 +2730,7 @@
       <c r="A242" t="s">
         <v>36</v>
       </c>
-      <c r="B242">
+      <c r="B242" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2725,7 +2738,7 @@
       <c r="A243" t="s">
         <v>43</v>
       </c>
-      <c r="B243">
+      <c r="B243" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2733,7 +2746,7 @@
       <c r="A244" t="s">
         <v>80</v>
       </c>
-      <c r="B244">
+      <c r="B244" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2741,7 +2754,7 @@
       <c r="A245" t="s">
         <v>81</v>
       </c>
-      <c r="B245">
+      <c r="B245" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2749,7 +2762,7 @@
       <c r="A246" t="s">
         <v>82</v>
       </c>
-      <c r="B246">
+      <c r="B246" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2757,7 +2770,7 @@
       <c r="A247" t="s">
         <v>83</v>
       </c>
-      <c r="B247">
+      <c r="B247" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2765,7 +2778,7 @@
       <c r="A248" t="s">
         <v>84</v>
       </c>
-      <c r="B248">
+      <c r="B248" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2773,7 +2786,7 @@
       <c r="A249" t="s">
         <v>85</v>
       </c>
-      <c r="B249">
+      <c r="B249" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2781,7 +2794,7 @@
       <c r="A250" t="s">
         <v>86</v>
       </c>
-      <c r="B250">
+      <c r="B250" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2789,7 +2802,7 @@
       <c r="A251" t="s">
         <v>87</v>
       </c>
-      <c r="B251">
+      <c r="B251" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2797,7 +2810,7 @@
       <c r="A252" t="s">
         <v>56</v>
       </c>
-      <c r="B252">
+      <c r="B252" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2805,7 +2818,7 @@
       <c r="A253" t="s">
         <v>88</v>
       </c>
-      <c r="B253">
+      <c r="B253" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2813,7 +2826,7 @@
       <c r="A254" t="s">
         <v>89</v>
       </c>
-      <c r="B254">
+      <c r="B254" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2821,7 +2834,7 @@
       <c r="A255" t="s">
         <v>89</v>
       </c>
-      <c r="B255">
+      <c r="B255" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2829,7 +2842,7 @@
       <c r="A256" t="s">
         <v>88</v>
       </c>
-      <c r="B256">
+      <c r="B256" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2837,7 +2850,7 @@
       <c r="A257" t="s">
         <v>90</v>
       </c>
-      <c r="B257">
+      <c r="B257" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2845,7 +2858,7 @@
       <c r="A258" t="s">
         <v>88</v>
       </c>
-      <c r="B258">
+      <c r="B258" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2853,7 +2866,7 @@
       <c r="A259" t="s">
         <v>91</v>
       </c>
-      <c r="B259">
+      <c r="B259" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2861,7 +2874,7 @@
       <c r="A260" t="s">
         <v>91</v>
       </c>
-      <c r="B260">
+      <c r="B260" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2869,7 +2882,7 @@
       <c r="A261" t="s">
         <v>92</v>
       </c>
-      <c r="B261">
+      <c r="B261" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2877,7 +2890,7 @@
       <c r="A262" t="s">
         <v>92</v>
       </c>
-      <c r="B262">
+      <c r="B262" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2885,7 +2898,7 @@
       <c r="A263" t="s">
         <v>92</v>
       </c>
-      <c r="B263">
+      <c r="B263" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2893,7 +2906,7 @@
       <c r="A264" t="s">
         <v>92</v>
       </c>
-      <c r="B264">
+      <c r="B264" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2901,7 +2914,7 @@
       <c r="A265" t="s">
         <v>93</v>
       </c>
-      <c r="B265">
+      <c r="B265" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2909,7 +2922,7 @@
       <c r="A266" t="s">
         <v>94</v>
       </c>
-      <c r="B266">
+      <c r="B266" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2917,7 +2930,7 @@
       <c r="A267" t="s">
         <v>94</v>
       </c>
-      <c r="B267">
+      <c r="B267" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2925,7 +2938,7 @@
       <c r="A268" t="s">
         <v>93</v>
       </c>
-      <c r="B268">
+      <c r="B268" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2933,7 +2946,7 @@
       <c r="A269" t="s">
         <v>95</v>
       </c>
-      <c r="B269">
+      <c r="B269" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2941,7 +2954,7 @@
       <c r="A270" t="s">
         <v>96</v>
       </c>
-      <c r="B270">
+      <c r="B270" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2949,7 +2962,7 @@
       <c r="A271" t="s">
         <v>97</v>
       </c>
-      <c r="B271">
+      <c r="B271" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2957,7 +2970,7 @@
       <c r="A272" t="s">
         <v>98</v>
       </c>
-      <c r="B272">
+      <c r="B272" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2965,7 +2978,7 @@
       <c r="A273" t="s">
         <v>99</v>
       </c>
-      <c r="B273">
+      <c r="B273" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2973,7 +2986,7 @@
       <c r="A274" t="s">
         <v>100</v>
       </c>
-      <c r="B274">
+      <c r="B274" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2981,7 +2994,7 @@
       <c r="A275" t="s">
         <v>101</v>
       </c>
-      <c r="B275">
+      <c r="B275" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2989,7 +3002,7 @@
       <c r="A276" t="s">
         <v>102</v>
       </c>
-      <c r="B276">
+      <c r="B276" s="1">
         <v>200</v>
       </c>
     </row>
@@ -2997,7 +3010,7 @@
       <c r="A277" t="s">
         <v>103</v>
       </c>
-      <c r="B277">
+      <c r="B277" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3005,7 +3018,7 @@
       <c r="A278" t="s">
         <v>104</v>
       </c>
-      <c r="B278">
+      <c r="B278" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3013,7 +3026,7 @@
       <c r="A279" t="s">
         <v>104</v>
       </c>
-      <c r="B279">
+      <c r="B279" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3021,7 +3034,7 @@
       <c r="A280" t="s">
         <v>105</v>
       </c>
-      <c r="B280">
+      <c r="B280" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3029,7 +3042,7 @@
       <c r="A281" t="s">
         <v>106</v>
       </c>
-      <c r="B281">
+      <c r="B281" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3037,7 +3050,7 @@
       <c r="A282" t="s">
         <v>72</v>
       </c>
-      <c r="B282">
+      <c r="B282" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3045,7 +3058,7 @@
       <c r="A283" t="s">
         <v>107</v>
       </c>
-      <c r="B283">
+      <c r="B283" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3053,7 +3066,7 @@
       <c r="A284" t="s">
         <v>108</v>
       </c>
-      <c r="B284">
+      <c r="B284" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3061,7 +3074,7 @@
       <c r="A285" t="s">
         <v>109</v>
       </c>
-      <c r="B285">
+      <c r="B285" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3069,7 +3082,7 @@
       <c r="A286" t="s">
         <v>110</v>
       </c>
-      <c r="B286">
+      <c r="B286" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3077,7 +3090,7 @@
       <c r="A287" t="s">
         <v>111</v>
       </c>
-      <c r="B287">
+      <c r="B287" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3085,7 +3098,7 @@
       <c r="A288" t="s">
         <v>112</v>
       </c>
-      <c r="B288">
+      <c r="B288" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3093,7 +3106,7 @@
       <c r="A289" t="s">
         <v>113</v>
       </c>
-      <c r="B289">
+      <c r="B289" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3101,7 +3114,7 @@
       <c r="A290" t="s">
         <v>114</v>
       </c>
-      <c r="B290">
+      <c r="B290" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3109,7 +3122,7 @@
       <c r="A291" t="s">
         <v>115</v>
       </c>
-      <c r="B291">
+      <c r="B291" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3117,7 +3130,7 @@
       <c r="A292" t="s">
         <v>116</v>
       </c>
-      <c r="B292">
+      <c r="B292" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3125,7 +3138,7 @@
       <c r="A293" t="s">
         <v>117</v>
       </c>
-      <c r="B293">
+      <c r="B293" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3133,7 +3146,7 @@
       <c r="A294" t="s">
         <v>118</v>
       </c>
-      <c r="B294">
+      <c r="B294" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3141,7 +3154,7 @@
       <c r="A295" t="s">
         <v>117</v>
       </c>
-      <c r="B295">
+      <c r="B295" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3149,7 +3162,7 @@
       <c r="A296" t="s">
         <v>118</v>
       </c>
-      <c r="B296">
+      <c r="B296" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3157,7 +3170,7 @@
       <c r="A297" t="s">
         <v>119</v>
       </c>
-      <c r="B297">
+      <c r="B297" s="1">
         <v>200</v>
       </c>
     </row>
@@ -3165,17 +3178,20 @@
       <c r="A298" t="s">
         <v>120</v>
       </c>
-      <c r="B298">
-        <v>200</v>
+      <c r="B298" s="1">
+        <v>404</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>121</v>
       </c>
-      <c r="B299">
-        <v>200</v>
-      </c>
+      <c r="B299" s="1">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A304" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>